<commit_message>
VS-161. Add support for lots of hotkeys. Still more to go. Also, canvas navigation is still to come. See the spreadsheet for progress. Green rows are implemented, white is unimplemented, orange means that particular feature is not implemented yet, and red means unity has reserved those hotkeys and we have no way to intercept them. Coolest hotkey so far => <space> - it removes the utility panels so that the graph portion takes up the whole window - great idea whoever came up with it! :)
git-svn-id: https://www.detoxstudios.com/projectdepot/Development/Unity@499 b191eb17-2330-428c-a13f-159e02ee8e09
</commit_message>
<xml_diff>
--- a/uScript_Dev/Documents/Usability_Input_List.xlsx
+++ b/uScript_Dev/Documents/Usability_Input_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13780" yWindow="0" windowWidth="20200" windowHeight="22560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="13785" yWindow="0" windowWidth="20205" windowHeight="15990" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hot-Keys" sheetId="1" r:id="rId1"/>
     <sheet name="GUI Functionality" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="153">
   <si>
     <t>Place External Connection node where clicked</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -656,17 +656,14 @@
     <t>]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>CTRL + SHIFT+ S</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -687,12 +684,36 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -707,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -746,6 +767,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1075,27 +1120,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:I67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.125" customWidth="1"/>
+    <col min="2" max="2" width="40.375" customWidth="1"/>
+    <col min="3" max="3" width="15.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" ht="16">
+    <row r="4" spans="2:9" ht="15">
       <c r="B4" s="2" t="s">
         <v>112</v>
       </c>
@@ -1131,113 +1176,165 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="2:9" s="17" customFormat="1">
+      <c r="B7" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="2:9" s="17" customFormat="1">
+      <c r="B8" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="C8" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="2:9" s="20" customFormat="1">
+      <c r="B9" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="2:9" s="20" customFormat="1">
+      <c r="B10" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="2:9" s="20" customFormat="1">
+      <c r="B11" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="2:9" s="20" customFormat="1">
+      <c r="B12" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="2:9" s="20" customFormat="1">
+      <c r="B13" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
-      <c r="B14" s="3" t="s">
+    <row r="14" spans="2:9" s="17" customFormat="1">
+      <c r="B14" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="2:9" s="17" customFormat="1">
+      <c r="B15" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="2:9" s="20" customFormat="1">
+      <c r="B16" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1286,61 +1383,77 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
-      <c r="B25" s="3" t="s">
+    <row r="25" spans="2:9" s="23" customFormat="1">
+      <c r="B25" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
-      <c r="B26" s="3" t="s">
+    <row r="26" spans="2:9" s="23" customFormat="1">
+      <c r="B26" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
-      <c r="B27" s="3" t="s">
+    <row r="27" spans="2:9" s="23" customFormat="1">
+      <c r="B27" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
-      <c r="B28" s="3" t="s">
+    <row r="28" spans="2:9" s="20" customFormat="1">
+      <c r="B28" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="19" t="s">
         <v>96</v>
       </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="3" t="s">
@@ -1350,32 +1463,49 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="2:9">
-      <c r="B30" s="3" t="s">
+    <row r="30" spans="2:9" s="20" customFormat="1">
+      <c r="B30" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="31" spans="2:9">
-      <c r="B31" s="3" t="s">
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+    </row>
+    <row r="31" spans="2:9" s="23" customFormat="1">
+      <c r="B31" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:9">
-      <c r="B32" s="3" t="s">
+    <row r="32" spans="2:9" s="20" customFormat="1">
+      <c r="B32" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="19" t="s">
         <v>103</v>
       </c>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="3" t="s">
@@ -1393,38 +1523,53 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
-      <c r="B35" s="3" t="s">
+    <row r="35" spans="2:9" s="20" customFormat="1">
+      <c r="B35" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="19" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="36" spans="2:9">
-      <c r="B36" s="3" t="s">
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+    </row>
+    <row r="36" spans="2:9" s="20" customFormat="1">
+      <c r="B36" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
-      <c r="B37" s="3" t="s">
+    <row r="37" spans="2:9" s="20" customFormat="1">
+      <c r="B37" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="D37" s="19"/>
+      <c r="E37" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="F37" s="19"/>
+      <c r="G37" s="19" t="s">
         <v>28</v>
       </c>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
     </row>
     <row r="38" spans="2:9">
       <c r="B38" s="3" t="s">
@@ -1434,21 +1579,33 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
-      <c r="B39" s="3" t="s">
+    <row r="39" spans="2:9" s="23" customFormat="1">
+      <c r="B39" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="22" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="40" spans="2:9">
-      <c r="B40" s="3" t="s">
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+    </row>
+    <row r="40" spans="2:9" s="23" customFormat="1">
+      <c r="B40" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="22" t="s">
         <v>57</v>
       </c>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
     </row>
     <row r="41" spans="2:9">
       <c r="B41" s="3" t="s">
@@ -1666,31 +1823,39 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="2:9">
-      <c r="B59" s="3" t="s">
+    <row r="59" spans="2:9" s="23" customFormat="1">
+      <c r="B59" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="I59" s="6" t="s">
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="22" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="2:9">
-      <c r="B60" s="3" t="s">
+    <row r="60" spans="2:9" s="23" customFormat="1">
+      <c r="B60" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="I60" s="6" t="s">
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1710,10 +1875,9 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1723,23 +1887,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="14" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="8"/>
+    <col min="1" max="1" width="3.375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" style="14" customWidth="1"/>
+    <col min="4" max="4" width="61.25" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="10.75" style="8"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" ht="16">
+    <row r="4" spans="2:4" ht="15">
       <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
@@ -1782,7 +1946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="39">
+    <row r="9" spans="2:4" ht="38.25">
       <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
@@ -1794,7 +1958,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
VS-161. Implement new mouse control. Update usability chart completion status. Only a few more small items to go!
git-svn-id: https://www.detoxstudios.com/projectdepot/Development/Unity@510 b191eb17-2330-428c-a13f-159e02ee8e09
</commit_message>
<xml_diff>
--- a/uScript_Dev/Documents/Usability_Input_List.xlsx
+++ b/uScript_Dev/Documents/Usability_Input_List.xlsx
@@ -1123,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -1571,13 +1571,19 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="2:9">
-      <c r="B38" s="3" t="s">
+    <row r="38" spans="2:9" s="20" customFormat="1">
+      <c r="B38" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="19" t="s">
         <v>63</v>
       </c>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
     </row>
     <row r="39" spans="2:9" s="23" customFormat="1">
       <c r="B39" s="21" t="s">
@@ -1607,210 +1613,289 @@
       <c r="H40" s="22"/>
       <c r="I40" s="22"/>
     </row>
-    <row r="41" spans="2:9">
-      <c r="B41" s="3" t="s">
+    <row r="41" spans="2:9" s="20" customFormat="1">
+      <c r="B41" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="F41" s="19"/>
+      <c r="G41" s="19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="42" spans="2:9">
-      <c r="B42" s="3" t="s">
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+    </row>
+    <row r="42" spans="2:9" s="20" customFormat="1">
+      <c r="B42" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="F42" s="19"/>
+      <c r="G42" s="19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="43" spans="2:9">
-      <c r="B43" s="3" t="s">
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+    </row>
+    <row r="43" spans="2:9" s="20" customFormat="1">
+      <c r="B43" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="F43" s="19"/>
+      <c r="G43" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="44" spans="2:9">
-      <c r="B44" s="3" t="s">
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+    </row>
+    <row r="44" spans="2:9" s="20" customFormat="1">
+      <c r="B44" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G44" s="6" t="s">
+      <c r="F44" s="19"/>
+      <c r="G44" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="45" spans="2:9">
-      <c r="B45" s="3" t="s">
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+    </row>
+    <row r="45" spans="2:9" s="20" customFormat="1">
+      <c r="B45" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="F45" s="19"/>
+      <c r="G45" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="46" spans="2:9">
-      <c r="B46" s="3" t="s">
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+    </row>
+    <row r="46" spans="2:9" s="20" customFormat="1">
+      <c r="B46" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="F46" s="19"/>
+      <c r="G46" s="19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="47" spans="2:9">
-      <c r="B47" s="3" t="s">
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+    </row>
+    <row r="47" spans="2:9" s="20" customFormat="1">
+      <c r="B47" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="F47" s="19"/>
+      <c r="G47" s="19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="48" spans="2:9">
-      <c r="B48" s="3" t="s">
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+    </row>
+    <row r="48" spans="2:9" s="20" customFormat="1">
+      <c r="B48" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="F48" s="19"/>
+      <c r="G48" s="19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="49" spans="2:9">
-      <c r="B49" s="3" t="s">
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+    </row>
+    <row r="49" spans="2:9" s="20" customFormat="1">
+      <c r="B49" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="F49" s="19"/>
+      <c r="G49" s="19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="50" spans="2:9">
-      <c r="B50" s="3" t="s">
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+    </row>
+    <row r="50" spans="2:9" s="20" customFormat="1">
+      <c r="B50" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G50" s="6" t="s">
+      <c r="F50" s="19"/>
+      <c r="G50" s="19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="51" spans="2:9">
-      <c r="B51" s="3" t="s">
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+    </row>
+    <row r="51" spans="2:9" s="20" customFormat="1">
+      <c r="B51" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="F51" s="19"/>
+      <c r="G51" s="19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="52" spans="2:9">
-      <c r="B52" s="3" t="s">
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+    </row>
+    <row r="52" spans="2:9" s="20" customFormat="1">
+      <c r="B52" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G52" s="6" t="s">
+      <c r="F52" s="19"/>
+      <c r="G52" s="19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="53" spans="2:9">
-      <c r="B53" s="3" t="s">
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+    </row>
+    <row r="53" spans="2:9" s="20" customFormat="1">
+      <c r="B53" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G53" s="6" t="s">
+      <c r="F53" s="19"/>
+      <c r="G53" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H53" s="6" t="s">
+      <c r="H53" s="19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="54" spans="2:9">
-      <c r="B54" s="3" t="s">
+      <c r="I53" s="19"/>
+    </row>
+    <row r="54" spans="2:9" s="20" customFormat="1">
+      <c r="B54" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="G54" s="6" t="s">
+      <c r="F54" s="19"/>
+      <c r="G54" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H54" s="6" t="s">
+      <c r="H54" s="19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="55" spans="2:9">
-      <c r="B55" s="3" t="s">
+      <c r="I54" s="19"/>
+    </row>
+    <row r="55" spans="2:9" s="20" customFormat="1">
+      <c r="B55" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="G55" s="6" t="s">
+      <c r="F55" s="19"/>
+      <c r="G55" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="H55" s="19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="56" spans="2:9">
-      <c r="B56" s="3" t="s">
+      <c r="I55" s="19"/>
+    </row>
+    <row r="56" spans="2:9" s="20" customFormat="1">
+      <c r="B56" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="F56" s="19"/>
+      <c r="G56" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="H56" s="19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="57" spans="2:9">
-      <c r="B57" s="3" t="s">
+      <c r="I56" s="19"/>
+    </row>
+    <row r="57" spans="2:9" s="20" customFormat="1">
+      <c r="B57" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="F57" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="G57" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H57" s="6" t="s">
+      <c r="H57" s="19" t="s">
         <v>93</v>
       </c>
+      <c r="I57" s="19"/>
     </row>
     <row r="58" spans="2:9">
       <c r="B58" s="3" t="s">

</xml_diff>

<commit_message>
VS-161. Backspace deletes selected items. Update spreadsheet adding it as an alt key.
git-svn-id: https://www.detoxstudios.com/projectdepot/Development/Unity@512 b191eb17-2330-428c-a13f-159e02ee8e09
</commit_message>
<xml_diff>
--- a/uScript_Dev/Documents/Usability_Input_List.xlsx
+++ b/uScript_Dev/Documents/Usability_Input_List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="154">
   <si>
     <t>Place External Connection node where clicked</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -181,10 +181,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CTRL + LMB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>LMB</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -658,6 +654,12 @@
   </si>
   <si>
     <t>CTRL + SHIFT+ S</t>
+  </si>
+  <si>
+    <t>BACKSPACE</t>
+  </si>
+  <si>
+    <t>SHIFT + LMB</t>
   </si>
 </sst>
 </file>
@@ -1123,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -1142,46 +1144,46 @@
   <sheetData>
     <row r="4" spans="2:9" ht="15">
       <c r="B4" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="G5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="2:9" s="17" customFormat="1">
       <c r="B7" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -1189,15 +1191,15 @@
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="2:9" s="17" customFormat="1">
       <c r="B8" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -1205,15 +1207,15 @@
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="2:9" s="20" customFormat="1">
       <c r="B9" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -1221,15 +1223,15 @@
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="2:9" s="20" customFormat="1">
       <c r="B10" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -1237,15 +1239,15 @@
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:9" s="20" customFormat="1">
       <c r="B11" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
@@ -1253,15 +1255,15 @@
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
       <c r="I11" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="2:9" s="20" customFormat="1">
       <c r="B12" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
@@ -1269,33 +1271,33 @@
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
       <c r="I12" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="2:9" s="20" customFormat="1">
       <c r="B13" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
       <c r="I13" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="2:9" s="17" customFormat="1">
       <c r="B14" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1303,15 +1305,15 @@
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="2:9" s="17" customFormat="1">
       <c r="B15" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1319,15 +1321,15 @@
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="2:9" s="20" customFormat="1">
       <c r="B16" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -1335,44 +1337,44 @@
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="22" spans="2:9">
       <c r="B22" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="23" spans="2:9">
@@ -1380,73 +1382,73 @@
     </row>
     <row r="24" spans="2:9">
       <c r="B24" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="2:9" s="23" customFormat="1">
       <c r="B25" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="D25" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="22" t="s">
-        <v>150</v>
-      </c>
       <c r="E25" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="2:9" s="23" customFormat="1">
       <c r="B26" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="2:9" s="23" customFormat="1">
       <c r="B27" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="D27" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="2:9" s="20" customFormat="1">
       <c r="B28" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
@@ -1457,20 +1459,22 @@
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="2:9" s="20" customFormat="1">
       <c r="B30" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="19"/>
+        <v>96</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>152</v>
+      </c>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
@@ -1479,10 +1483,10 @@
     </row>
     <row r="31" spans="2:9" s="23" customFormat="1">
       <c r="B31" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -1490,15 +1494,15 @@
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
       <c r="I31" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="2:9" s="20" customFormat="1">
       <c r="B32" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="19" t="s">
         <v>102</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>103</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
@@ -1509,26 +1513,26 @@
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="2:9">
       <c r="B34" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="35" spans="2:9" s="20" customFormat="1">
       <c r="B35" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
@@ -1539,10 +1543,10 @@
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1">
       <c r="B36" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
@@ -1550,19 +1554,19 @@
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
       <c r="I36" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="2:9" s="20" customFormat="1">
       <c r="B37" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F37" s="19"/>
       <c r="G37" s="19" t="s">
@@ -1573,10 +1577,10 @@
     </row>
     <row r="38" spans="2:9" s="20" customFormat="1">
       <c r="B38" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="19" t="s">
         <v>62</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>63</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
@@ -1587,10 +1591,10 @@
     </row>
     <row r="39" spans="2:9" s="23" customFormat="1">
       <c r="B39" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>64</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>65</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -1601,10 +1605,10 @@
     </row>
     <row r="40" spans="2:9" s="23" customFormat="1">
       <c r="B40" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="22" t="s">
         <v>56</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>57</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -1620,7 +1624,7 @@
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
       <c r="E41" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F41" s="19"/>
       <c r="G41" s="19" t="s">
@@ -1636,7 +1640,7 @@
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
       <c r="E42" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F42" s="19"/>
       <c r="G42" s="19" t="s">
@@ -1652,7 +1656,7 @@
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
       <c r="E43" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F43" s="19"/>
       <c r="G43" s="19" t="s">
@@ -1668,7 +1672,7 @@
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
       <c r="E44" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F44" s="19"/>
       <c r="G44" s="19" t="s">
@@ -1684,7 +1688,7 @@
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
       <c r="E45" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F45" s="19"/>
       <c r="G45" s="19" t="s">
@@ -1700,7 +1704,7 @@
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
       <c r="E46" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="19" t="s">
@@ -1716,7 +1720,7 @@
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
       <c r="E47" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F47" s="19"/>
       <c r="G47" s="19" t="s">
@@ -1732,7 +1736,7 @@
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
       <c r="E48" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F48" s="19"/>
       <c r="G48" s="19" t="s">
@@ -1748,7 +1752,7 @@
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
       <c r="E49" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F49" s="19"/>
       <c r="G49" s="19" t="s">
@@ -1764,7 +1768,7 @@
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
       <c r="E50" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F50" s="19"/>
       <c r="G50" s="19" t="s">
@@ -1775,7 +1779,7 @@
     </row>
     <row r="51" spans="2:9" s="20" customFormat="1">
       <c r="B51" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
@@ -1791,12 +1795,12 @@
     </row>
     <row r="52" spans="2:9" s="20" customFormat="1">
       <c r="B52" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C52" s="19"/>
       <c r="D52" s="19"/>
       <c r="E52" s="19" t="s">
-        <v>33</v>
+        <v>153</v>
       </c>
       <c r="F52" s="19"/>
       <c r="G52" s="19" t="s">
@@ -1807,19 +1811,19 @@
     </row>
     <row r="53" spans="2:9" s="20" customFormat="1">
       <c r="B53" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
       <c r="E53" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F53" s="19"/>
       <c r="G53" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H53" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I53" s="19"/>
     </row>
@@ -1830,14 +1834,14 @@
       <c r="C54" s="19"/>
       <c r="D54" s="19"/>
       <c r="E54" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F54" s="19"/>
       <c r="G54" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I54" s="19"/>
     </row>
@@ -1848,61 +1852,61 @@
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
       <c r="E55" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F55" s="19"/>
       <c r="G55" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H55" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I55" s="19"/>
     </row>
     <row r="56" spans="2:9" s="20" customFormat="1">
       <c r="B56" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
       <c r="E56" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F56" s="19"/>
       <c r="G56" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I56" s="19"/>
     </row>
     <row r="57" spans="2:9" s="20" customFormat="1">
       <c r="B57" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
       <c r="E57" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G57" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F57" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G57" s="19" t="s">
-        <v>45</v>
-      </c>
       <c r="H57" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I57" s="19"/>
     </row>
     <row r="58" spans="2:9">
       <c r="B58" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>31</v>
@@ -1910,38 +1914,38 @@
     </row>
     <row r="59" spans="2:9" s="23" customFormat="1">
       <c r="B59" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E59" s="22"/>
       <c r="F59" s="22"/>
       <c r="G59" s="22"/>
       <c r="H59" s="22"/>
       <c r="I59" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="2:9" s="23" customFormat="1">
       <c r="B60" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E60" s="22"/>
       <c r="F60" s="22"/>
       <c r="G60" s="22"/>
       <c r="H60" s="22"/>
       <c r="I60" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="2:2">

</xml_diff>

<commit_message>
Updated Quick Start Guide to reflect changes in latest build. Made a sheet in the excel file for formating a hot-key chart for the Quick Start Guide.
git-svn-id: https://www.detoxstudios.com/projectdepot/Development/Unity@532 b191eb17-2330-428c-a13f-159e02ee8e09
</commit_message>
<xml_diff>
--- a/uScript_Dev/Documents/Usability_Input_List.xlsx
+++ b/uScript_Dev/Documents/Usability_Input_List.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13785" yWindow="0" windowWidth="20205" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="9420" yWindow="560" windowWidth="21960" windowHeight="22080" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hot-Keys" sheetId="1" r:id="rId1"/>
     <sheet name="GUI Functionality" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,754 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="237">
+  <si>
+    <t>CTRL + V</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Undo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + Z</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Redo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Close uScript</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + W</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Key</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mouse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Mouse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Context</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Canvas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Full screen canvas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPACE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete selected nodes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Select all nodes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Center canvas on next Event node</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Center canvas on previous Event node</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resets canvas to center (default position)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL+H</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deselect all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ESC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Toggle Grid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + G</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place String variable where clicked</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place Float variable where clicked</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place Bool variable where clicked</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place GameObject variable where clicked</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>G + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place Object variable where clicked</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>O + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place Comment node where clicked</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place External Connection where clicked</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place Log node where clicked</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>New node selection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Toggle node selection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marquee - New node selection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LMB + Drag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marquee - Add to selection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHIFT + LMB + Drag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marquee - Remove from selection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + LMB + Drag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Move node</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LMB + Drag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pan canvas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALT + LMB + Drag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MMB + Drag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C, N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Context Menu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place Vector3 variable where clicked</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place Int variable where clicked</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>I + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Key</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mouse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Mouse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Context</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cut</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + X</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Paste</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + X</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + V</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + Z</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + SHIFT + Z</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + O</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + W</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Panels</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focus on next control</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TAB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focus on previous control</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHIFT + TAB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commit changes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENTER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cancels changes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ESC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Canvas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoom out to next level</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + -</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + SHIFT+ S</t>
+  </si>
+  <si>
+    <t>BACKSPACE</t>
+  </si>
+  <si>
+    <t>SHIFT + LMB</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Previous breadcrumb nested level</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Next breadcrumb nested level</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PageUp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PageDown</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Show Detail View Window</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ESC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deselect all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Toggle Grid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + G</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Show Preferences Window</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + P</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>I + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>G + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>O + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>E + LMB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Toggle node selection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>New node selection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Marquee - New node selection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + =</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoom in to next level</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoom to 100% (default)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + 0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wheel Down</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wheel Up</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GUI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Save file as…</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Full screen canvas (hide panels)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPACE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focus on property grid for current selection</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete selected nodes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoom extends selection (all if no selection)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Select all nodes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Center canvas on next Event node</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Center canvas on previous Event node</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resets canvas to center (default position)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open online reference in default browser</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hot-Keys</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Save file</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cut</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Paste</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Undo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Redo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open file</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>New file</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Close uScript</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Action</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Key</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mouse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alt Mouse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTRL + S</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Place External Connection node where clicked</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -244,427 +992,18 @@
     <t>Double Click LMB</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
-  <si>
-    <t>,</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Previous breadcrumb nested level</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Next breadcrumb nested level</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PageUp</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PageDown</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Show Detail View Window</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + D</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>L + LMB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ESC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deselect all</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Toggle Grid</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + G</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Show Preferences Window</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + P</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>S + LMB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>V + LMB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>I + LMB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>F + LMB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>B + LMB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C + LMB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>G + LMB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>O + LMB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>E + LMB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Toggle node selection</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>New node selection</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Marquee - New node selection</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + =</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zoom in to next level</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zoom to 100% (default)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + 0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>\</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wheel Down</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wheel Up</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GUI</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Save file as…</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Full screen canvas (hide panels)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SPACE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DELETE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Focus on property grid for current selection</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Delete selected nodes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zoom extends selection (all if no selection)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Select all nodes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Center canvas on next Event node</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Center canvas on previous Event node</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>HOME</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resets canvas to center (default position)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>F1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open online reference in default browser</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hot-Keys</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Save file</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cut</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Copy</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Paste</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Undo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Redo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open file</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>New file</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Close uScript</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>General</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Action</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Key</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Alt Key</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mouse</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Alt Mouse</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + S</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + X</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + C</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + V</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + Y</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + Z</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + SHIFT + Z</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + N</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + O</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + W</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Panels</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Focus on next control</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TAB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Focus on previous control</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHIFT + TAB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commit changes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ENTER</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cancels changes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ESC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Canvas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zoom out to next level</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + -</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>[</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTRL + SHIFT+ S</t>
-  </si>
-  <si>
-    <t>BACKSPACE</t>
-  </si>
-  <si>
-    <t>SHIFT + LMB</t>
-  </si>
-  <si>
-    <t>]</t>
-  </si>
-  <si>
-    <t>[</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -683,8 +1022,19 @@
       <sz val="12"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="53"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -715,6 +1065,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -728,7 +1090,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -790,6 +1152,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1120,68 +1496,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="B4:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:I67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="3.125" customWidth="1"/>
-    <col min="2" max="2" width="40.375" customWidth="1"/>
-    <col min="3" max="3" width="15.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" ht="15">
+    <row r="4" spans="2:9" ht="16">
       <c r="B4" s="2" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="5" t="s">
-        <v>120</v>
+        <v>182</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>121</v>
+        <v>183</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>122</v>
+        <v>184</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>124</v>
+        <v>186</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>34</v>
+        <v>222</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>45</v>
+        <v>233</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="1" t="s">
-        <v>119</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="2:9" s="17" customFormat="1">
       <c r="B7" s="15" t="s">
-        <v>110</v>
+        <v>172</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -1189,15 +1565,15 @@
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16" t="s">
-        <v>89</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="2:9" s="17" customFormat="1">
       <c r="B8" s="15" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -1205,15 +1581,15 @@
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16" t="s">
-        <v>91</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="2:9" s="20" customFormat="1">
       <c r="B9" s="18" t="s">
-        <v>111</v>
+        <v>173</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -1221,15 +1597,15 @@
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19" t="s">
-        <v>87</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="2:9" s="20" customFormat="1">
       <c r="B10" s="18" t="s">
-        <v>112</v>
+        <v>174</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -1237,15 +1613,15 @@
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19" t="s">
-        <v>87</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="2:9" s="20" customFormat="1">
       <c r="B11" s="18" t="s">
-        <v>113</v>
+        <v>175</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
@@ -1253,15 +1629,15 @@
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
       <c r="I11" s="19" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="2:9" s="20" customFormat="1">
       <c r="B12" s="18" t="s">
-        <v>114</v>
+        <v>176</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
@@ -1269,33 +1645,33 @@
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
       <c r="I12" s="19" t="s">
-        <v>89</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="2:9" s="20" customFormat="1">
       <c r="B13" s="18" t="s">
-        <v>115</v>
+        <v>177</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
       <c r="I13" s="19" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="2:9" s="17" customFormat="1">
       <c r="B14" s="15" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1303,15 +1679,15 @@
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="2:9" s="17" customFormat="1">
       <c r="B15" s="15" t="s">
-        <v>116</v>
+        <v>178</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1319,15 +1695,15 @@
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16" t="s">
-        <v>87</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="2:9" s="20" customFormat="1">
       <c r="B16" s="18" t="s">
-        <v>118</v>
+        <v>180</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -1335,44 +1711,44 @@
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19" t="s">
-        <v>88</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="4" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="3" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="3" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="3" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="2:9">
       <c r="B22" s="3" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="2:9">
@@ -1380,73 +1756,73 @@
     </row>
     <row r="24" spans="2:9">
       <c r="B24" s="4" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="2:9" s="23" customFormat="1">
       <c r="B25" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="22" t="s">
         <v>145</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22" t="s">
-        <v>93</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="2:9" s="23" customFormat="1">
       <c r="B26" s="21" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>84</v>
+        <v>146</v>
       </c>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="2:9" s="23" customFormat="1">
       <c r="B27" s="21" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22" t="s">
-        <v>88</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="2:9" s="20" customFormat="1">
       <c r="B28" s="18" t="s">
-        <v>94</v>
+        <v>156</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
@@ -1457,21 +1833,21 @@
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="30" spans="2:9" s="20" customFormat="1">
       <c r="B30" s="18" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
@@ -1481,10 +1857,10 @@
     </row>
     <row r="31" spans="2:9" s="23" customFormat="1">
       <c r="B31" s="21" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -1492,15 +1868,15 @@
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
       <c r="I31" s="22" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="2:9" s="20" customFormat="1">
       <c r="B32" s="18" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
@@ -1511,10 +1887,10 @@
     </row>
     <row r="33" spans="2:9" s="20" customFormat="1">
       <c r="B33" s="18" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
@@ -1525,10 +1901,10 @@
     </row>
     <row r="34" spans="2:9" s="20" customFormat="1">
       <c r="B34" s="18" t="s">
-        <v>104</v>
+        <v>166</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
@@ -1539,10 +1915,10 @@
     </row>
     <row r="35" spans="2:9" s="20" customFormat="1">
       <c r="B35" s="18" t="s">
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
@@ -1553,10 +1929,10 @@
     </row>
     <row r="36" spans="2:9" s="20" customFormat="1">
       <c r="B36" s="18" t="s">
-        <v>108</v>
+        <v>170</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>107</v>
+        <v>169</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
@@ -1564,33 +1940,33 @@
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
       <c r="I36" s="19" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="2:9" s="20" customFormat="1">
       <c r="B37" s="18" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="19" t="s">
-        <v>33</v>
+        <v>221</v>
       </c>
       <c r="F37" s="19"/>
       <c r="G37" s="19" t="s">
-        <v>28</v>
+        <v>216</v>
       </c>
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
     </row>
     <row r="38" spans="2:9" s="20" customFormat="1">
       <c r="B38" s="18" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
@@ -1601,10 +1977,10 @@
     </row>
     <row r="39" spans="2:9" s="23" customFormat="1">
       <c r="B39" s="21" t="s">
-        <v>63</v>
+        <v>125</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
@@ -1615,10 +1991,10 @@
     </row>
     <row r="40" spans="2:9" s="23" customFormat="1">
       <c r="B40" s="21" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
@@ -1629,354 +2005,355 @@
     </row>
     <row r="41" spans="2:9" s="20" customFormat="1">
       <c r="B41" s="18" t="s">
-        <v>18</v>
+        <v>206</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
       <c r="E41" s="19" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="F41" s="19"/>
       <c r="G41" s="19" t="s">
-        <v>29</v>
+        <v>217</v>
       </c>
       <c r="H41" s="19"/>
       <c r="I41" s="19"/>
     </row>
     <row r="42" spans="2:9" s="20" customFormat="1">
       <c r="B42" s="18" t="s">
-        <v>19</v>
+        <v>207</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
       <c r="E42" s="19" t="s">
-        <v>67</v>
+        <v>129</v>
       </c>
       <c r="F42" s="19"/>
       <c r="G42" s="19" t="s">
-        <v>29</v>
+        <v>217</v>
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="19"/>
     </row>
     <row r="43" spans="2:9" s="20" customFormat="1">
       <c r="B43" s="18" t="s">
-        <v>20</v>
+        <v>208</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
       <c r="E43" s="19" t="s">
-        <v>68</v>
+        <v>130</v>
       </c>
       <c r="F43" s="19"/>
       <c r="G43" s="19" t="s">
-        <v>28</v>
+        <v>216</v>
       </c>
       <c r="H43" s="19"/>
       <c r="I43" s="19"/>
     </row>
     <row r="44" spans="2:9" s="20" customFormat="1">
       <c r="B44" s="18" t="s">
-        <v>21</v>
+        <v>209</v>
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
       <c r="E44" s="19" t="s">
-        <v>69</v>
+        <v>131</v>
       </c>
       <c r="F44" s="19"/>
       <c r="G44" s="19" t="s">
-        <v>28</v>
+        <v>216</v>
       </c>
       <c r="H44" s="19"/>
       <c r="I44" s="19"/>
     </row>
     <row r="45" spans="2:9" s="20" customFormat="1">
       <c r="B45" s="18" t="s">
-        <v>22</v>
+        <v>210</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
       <c r="E45" s="19" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="F45" s="19"/>
       <c r="G45" s="19" t="s">
-        <v>28</v>
+        <v>216</v>
       </c>
       <c r="H45" s="19"/>
       <c r="I45" s="19"/>
     </row>
     <row r="46" spans="2:9" s="20" customFormat="1">
       <c r="B46" s="18" t="s">
-        <v>23</v>
+        <v>211</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
       <c r="E46" s="19" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="19" t="s">
-        <v>29</v>
+        <v>217</v>
       </c>
       <c r="H46" s="19"/>
       <c r="I46" s="19"/>
     </row>
     <row r="47" spans="2:9" s="20" customFormat="1">
       <c r="B47" s="18" t="s">
-        <v>24</v>
+        <v>212</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
       <c r="E47" s="19" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="F47" s="19"/>
       <c r="G47" s="19" t="s">
-        <v>29</v>
+        <v>217</v>
       </c>
       <c r="H47" s="19"/>
       <c r="I47" s="19"/>
     </row>
     <row r="48" spans="2:9" s="20" customFormat="1">
       <c r="B48" s="18" t="s">
-        <v>25</v>
+        <v>213</v>
       </c>
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
       <c r="E48" s="19" t="s">
-        <v>71</v>
+        <v>133</v>
       </c>
       <c r="F48" s="19"/>
       <c r="G48" s="19" t="s">
-        <v>29</v>
+        <v>217</v>
       </c>
       <c r="H48" s="19"/>
       <c r="I48" s="19"/>
     </row>
     <row r="49" spans="2:9" s="20" customFormat="1">
       <c r="B49" s="18" t="s">
-        <v>0</v>
+        <v>188</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
       <c r="E49" s="19" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="F49" s="19"/>
       <c r="G49" s="19" t="s">
-        <v>28</v>
+        <v>216</v>
       </c>
       <c r="H49" s="19"/>
       <c r="I49" s="19"/>
     </row>
     <row r="50" spans="2:9" s="20" customFormat="1">
       <c r="B50" s="18" t="s">
-        <v>1</v>
+        <v>189</v>
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
       <c r="E50" s="19" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="F50" s="19"/>
       <c r="G50" s="19" t="s">
-        <v>29</v>
+        <v>217</v>
       </c>
       <c r="H50" s="19"/>
       <c r="I50" s="19"/>
     </row>
     <row r="51" spans="2:9" s="20" customFormat="1">
       <c r="B51" s="18" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
       <c r="E51" s="19" t="s">
-        <v>32</v>
+        <v>220</v>
       </c>
       <c r="F51" s="19"/>
       <c r="G51" s="19" t="s">
-        <v>30</v>
+        <v>218</v>
       </c>
       <c r="H51" s="19"/>
       <c r="I51" s="19"/>
     </row>
     <row r="52" spans="2:9" s="20" customFormat="1">
       <c r="B52" s="18" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="C52" s="19"/>
       <c r="D52" s="19"/>
       <c r="E52" s="19" t="s">
-        <v>151</v>
+        <v>108</v>
       </c>
       <c r="F52" s="19"/>
       <c r="G52" s="19" t="s">
-        <v>31</v>
+        <v>219</v>
       </c>
       <c r="H52" s="19"/>
       <c r="I52" s="19"/>
     </row>
     <row r="53" spans="2:9" s="20" customFormat="1">
       <c r="B53" s="18" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
       <c r="E53" s="19" t="s">
-        <v>35</v>
+        <v>223</v>
       </c>
       <c r="F53" s="19"/>
       <c r="G53" s="19" t="s">
-        <v>36</v>
+        <v>224</v>
       </c>
       <c r="H53" s="19" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="I53" s="19"/>
     </row>
     <row r="54" spans="2:9" s="20" customFormat="1">
       <c r="B54" s="18" t="s">
-        <v>26</v>
+        <v>214</v>
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="19"/>
       <c r="E54" s="19" t="s">
-        <v>37</v>
+        <v>225</v>
       </c>
       <c r="F54" s="19"/>
       <c r="G54" s="19" t="s">
-        <v>38</v>
+        <v>226</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="I54" s="19"/>
     </row>
     <row r="55" spans="2:9" s="20" customFormat="1">
       <c r="B55" s="18" t="s">
-        <v>27</v>
+        <v>215</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
       <c r="E55" s="19" t="s">
-        <v>39</v>
+        <v>227</v>
       </c>
       <c r="F55" s="19"/>
       <c r="G55" s="19" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="H55" s="19" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="I55" s="19"/>
     </row>
     <row r="56" spans="2:9" s="20" customFormat="1">
       <c r="B56" s="18" t="s">
-        <v>40</v>
+        <v>228</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
       <c r="E56" s="19" t="s">
-        <v>35</v>
+        <v>223</v>
       </c>
       <c r="F56" s="19"/>
       <c r="G56" s="19" t="s">
-        <v>41</v>
+        <v>229</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="I56" s="19"/>
     </row>
     <row r="57" spans="2:9" s="20" customFormat="1">
       <c r="B57" s="18" t="s">
-        <v>42</v>
+        <v>230</v>
       </c>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
       <c r="E57" s="19" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>46</v>
+        <v>234</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>44</v>
+        <v>232</v>
       </c>
       <c r="H57" s="19" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="I57" s="19"/>
     </row>
     <row r="58" spans="2:9">
       <c r="B58" s="3" t="s">
-        <v>47</v>
+        <v>235</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>48</v>
+        <v>236</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>31</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="2:9" s="23" customFormat="1">
       <c r="B59" s="21" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="E59" s="22"/>
       <c r="F59" s="22"/>
       <c r="G59" s="22"/>
       <c r="H59" s="22"/>
       <c r="I59" s="22" t="s">
-        <v>88</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="2:9" s="23" customFormat="1">
       <c r="B60" s="21" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="E60" s="22"/>
       <c r="F60" s="22"/>
       <c r="G60" s="22"/>
       <c r="H60" s="22"/>
       <c r="I60" s="22" t="s">
-        <v>88</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="1" t="s">
-        <v>16</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="1" t="s">
-        <v>15</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="1" t="s">
-        <v>17</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1986,77 +2363,658 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="B4:D9"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="19.25" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.75" style="14" customWidth="1"/>
-    <col min="4" max="4" width="61.25" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="10.75" style="8"/>
+    <col min="1" max="1" width="3.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="10.7109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" ht="15">
+    <row r="4" spans="2:4" ht="16">
       <c r="B4" s="7" t="s">
-        <v>10</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="10" t="s">
-        <v>2</v>
+        <v>190</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>5</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="12" t="s">
-        <v>3</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="13" t="s">
-        <v>14</v>
+        <v>202</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>13</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="39">
+      <c r="B9" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="B5:G47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:7">
+      <c r="B5" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="38.25">
-      <c r="B9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="G14" s="26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="29"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>